<commit_message>
All results categorized and cleaned up
</commit_message>
<xml_diff>
--- a/experiments/human_evaluations/five_answer_best_context_concat_human_eval.xlsx
+++ b/experiments/human_evaluations/five_answer_best_context_concat_human_eval.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhysb\Git_Repositories\iTA\experiments\human_evaluations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhysb\Git_Repositories\iLFQA\experiments\human_evaluations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C7C228-FB98-4BEE-B9D2-BFC0F7A9119C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EC6334-B7FA-4295-9CDA-1D45FB674264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2252,7 +2252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -4425,7 +4425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="405" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>190</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="405" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>195</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="360" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="345" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>239</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="405" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="390" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>255</v>
       </c>
@@ -7725,8 +7725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD081FEC-996E-4CE6-AC80-F09D68C6AACF}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>